<commit_message>
add moirai distillation code
</commit_message>
<xml_diff>
--- a/summary_results.xlsx
+++ b/summary_results.xlsx
@@ -528,13 +528,13 @@
         <v>96</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5061771442504648</v>
+        <v>0.499594515336062</v>
       </c>
       <c r="G2" t="n">
-        <v>0.5456720430907108</v>
+        <v>0.5457157658167963</v>
       </c>
       <c r="H2" t="n">
-        <v>0.7114612738937129</v>
+        <v>0.7068200020769517</v>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="n">
@@ -548,12 +548,12 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>20260113_090057</t>
+          <t>20260114_222756</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>log/eval_results_student_final_model_ctx720_pred96_ETT-small_ETTh1_20260113_090057.json</t>
+          <t>log/eval_results_student_final_model_ctx720_pred96_ETT-small_ETTh1_20260114_222756.json</t>
         </is>
       </c>
     </row>
@@ -580,16 +580,16 @@
         <v>96</v>
       </c>
       <c r="F3" t="n">
-        <v>0.318130092896883</v>
+        <v>0.2881763828719404</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4332630098046857</v>
+        <v>0.4162601875924979</v>
       </c>
       <c r="H3" t="n">
-        <v>0.5640302233895653</v>
+        <v>0.536820624484511</v>
       </c>
       <c r="I3" t="n">
-        <v>33.612446007444</v>
+        <v>31.39830108526041</v>
       </c>
       <c r="J3" t="n">
         <v>3389</v>
@@ -602,12 +602,12 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>20260113_090331</t>
+          <t>20260114_223041</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>log/eval_results_student_final_model_ctx720_pred96_ETT-small_ETTh2_20260113_090331.json</t>
+          <t>log/eval_results_student_final_model_ctx720_pred96_ETT-small_ETTh2_20260114_223041.json</t>
         </is>
       </c>
     </row>
@@ -634,13 +634,13 @@
         <v>96</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2886876451895189</v>
+        <v>0.2953531332215709</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4003942008768016</v>
+        <v>0.4032155977788479</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5372966082058577</v>
+        <v>0.5434640128118613</v>
       </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="n">
@@ -654,12 +654,12 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>20260113_091317</t>
+          <t>20260114_224120</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>log/eval_results_student_final_model_ctx720_pred96_ETT-small_ETTm1_20260113_091317.json</t>
+          <t>log/eval_results_student_final_model_ctx720_pred96_ETT-small_ETTm1_20260114_224120.json</t>
         </is>
       </c>
     </row>
@@ -686,16 +686,16 @@
         <v>96</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2862485401922321</v>
+        <v>0.3077747014869599</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4072578385399211</v>
+        <v>0.4219569885366005</v>
       </c>
       <c r="H5" t="n">
-        <v>0.535021999727331</v>
+        <v>0.5547744600168252</v>
       </c>
       <c r="I5" t="n">
-        <v>33.11160884841486</v>
+        <v>33.43812254872181</v>
       </c>
       <c r="J5" t="n">
         <v>13841</v>
@@ -708,12 +708,12 @@
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>20260113_092302</t>
+          <t>20260114_224549</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>log/eval_results_student_final_model_ctx720_pred96_ETT-small_ETTm2_20260113_092302.json</t>
+          <t>log/eval_results_student_final_model_ctx720_pred96_ETT-small_ETTm2_20260114_224549.json</t>
         </is>
       </c>
     </row>
@@ -740,16 +740,16 @@
         <v>96</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3112156612247711</v>
+        <v>0.3282837756101207</v>
       </c>
       <c r="G6" t="n">
-        <v>0.3993481179976328</v>
+        <v>0.4035846430740939</v>
       </c>
       <c r="H6" t="n">
-        <v>0.5578670641154316</v>
+        <v>0.5729605358225999</v>
       </c>
       <c r="I6" t="n">
-        <v>6.60313040796787</v>
+        <v>6.580494126167016</v>
       </c>
       <c r="J6" t="n">
         <v>5165</v>
@@ -762,12 +762,12 @@
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>20260113_085819</t>
+          <t>20260114_222511</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>log/eval_results_student_final_model_ctx720_pred96_electricity_electricity_20260113_085819.json</t>
+          <t>log/eval_results_student_final_model_ctx720_pred96_electricity_electricity_20260114_222511.json</t>
         </is>
       </c>
     </row>
@@ -794,16 +794,16 @@
         <v>96</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3305167089970784</v>
+        <v>0.3221413003769462</v>
       </c>
       <c r="G7" t="n">
-        <v>0.4421851922045729</v>
+        <v>0.4394647102623246</v>
       </c>
       <c r="H7" t="n">
-        <v>0.5749058261985857</v>
+        <v>0.5675749293062072</v>
       </c>
       <c r="I7" t="n">
-        <v>3.360327427691863</v>
+        <v>3.320067071027121</v>
       </c>
       <c r="J7" t="n">
         <v>1422</v>
@@ -816,12 +816,12 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>20260113_092416</t>
+          <t>20260114_224706</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>log/eval_results_student_final_model_ctx720_pred96_exchange_rate_exchange_rate_20260113_092416.json</t>
+          <t>log/eval_results_student_final_model_ctx720_pred96_exchange_rate_exchange_rate_20260114_224706.json</t>
         </is>
       </c>
     </row>
@@ -848,16 +848,16 @@
         <v>96</v>
       </c>
       <c r="F8" t="n">
-        <v>2.074348180425977</v>
+        <v>2.208746659050244</v>
       </c>
       <c r="G8" t="n">
-        <v>1.207377486942835</v>
+        <v>1.258872218043728</v>
       </c>
       <c r="H8" t="n">
-        <v>1.440259761440962</v>
+        <v>1.486185270768838</v>
       </c>
       <c r="I8" t="n">
-        <v>22.78641011054801</v>
+        <v>23.41767444414218</v>
       </c>
       <c r="J8" t="n">
         <v>98</v>
@@ -870,12 +870,12 @@
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>20260113_092440</t>
+          <t>20260114_224724</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>log/eval_results_student_final_model_ctx720_pred96_illness_national_illness_20260113_092440.json</t>
+          <t>log/eval_results_student_final_model_ctx720_pred96_illness_national_illness_20260114_224724.json</t>
         </is>
       </c>
     </row>
@@ -902,13 +902,13 @@
         <v>96</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1808132486821951</v>
+        <v>0.1452621437960376</v>
       </c>
       <c r="G9" t="n">
-        <v>0.2980116770165426</v>
+        <v>0.2624838237040554</v>
       </c>
       <c r="H9" t="n">
-        <v>0.4252214113637683</v>
+        <v>0.3811327115271498</v>
       </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="n">
@@ -922,12 +922,12 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>20260113_093224</t>
+          <t>20260114_225419</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>log/eval_results_student_final_model_ctx720_pred96_traffic_traffic_20260113_093224.json</t>
+          <t>log/eval_results_student_final_model_ctx720_pred96_traffic_traffic_20260114_225419.json</t>
         </is>
       </c>
     </row>
@@ -954,16 +954,16 @@
         <v>96</v>
       </c>
       <c r="F10" t="n">
-        <v>0.5180811520683879</v>
+        <v>0.5215339690703901</v>
       </c>
       <c r="G10" t="n">
-        <v>0.5079028971440632</v>
+        <v>0.5080603164753477</v>
       </c>
       <c r="H10" t="n">
-        <v>0.7197785437677258</v>
+        <v>0.7221730880269563</v>
       </c>
       <c r="I10" t="n">
-        <v>1.910977897651677</v>
+        <v>1.907998342484382</v>
       </c>
       <c r="J10" t="n">
         <v>10444</v>
@@ -976,12 +976,12 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>20260113_093950</t>
+          <t>20260114_230213</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>log/eval_results_student_final_model_ctx720_pred96_weather_weather_20260113_093950.json</t>
+          <t>log/eval_results_student_final_model_ctx720_pred96_weather_weather_20260114_230213.json</t>
         </is>
       </c>
     </row>
@@ -1028,12 +1028,12 @@
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>20260113_085958</t>
+          <t>20260114_222648</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>log/eval_results_teacher_chronos-2_ctx720_pred96_ETT-small_ETTh1_20260113_085958.json</t>
+          <t>log/eval_results_teacher_chronos-2_ctx720_pred96_ETT-small_ETTh1_20260114_222648.json</t>
         </is>
       </c>
     </row>
@@ -1082,12 +1082,12 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>20260113_090235</t>
+          <t>20260114_222934</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>log/eval_results_teacher_chronos-2_ctx720_pred96_ETT-small_ETTh2_20260113_090235.json</t>
+          <t>log/eval_results_teacher_chronos-2_ctx720_pred96_ETT-small_ETTh2_20260114_222934.json</t>
         </is>
       </c>
     </row>
@@ -1134,12 +1134,12 @@
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>20260113_090946</t>
+          <t>20260114_223653</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>log/eval_results_teacher_chronos-2_ctx720_pred96_ETT-small_ETTm1_20260113_090946.json</t>
+          <t>log/eval_results_teacher_chronos-2_ctx720_pred96_ETT-small_ETTm1_20260114_223653.json</t>
         </is>
       </c>
     </row>
@@ -1242,12 +1242,12 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>20260113_085654</t>
+          <t>20260114_222327</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>log/eval_results_teacher_chronos-2_ctx720_pred96_electricity_electricity_20260113_085654.json</t>
+          <t>log/eval_results_teacher_chronos-2_ctx720_pred96_electricity_electricity_20260114_222327.json</t>
         </is>
       </c>
     </row>
@@ -1296,12 +1296,12 @@
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>20260113_092347</t>
+          <t>20260114_224634</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>log/eval_results_teacher_chronos-2_ctx720_pred96_exchange_rate_exchange_rate_20260113_092347.json</t>
+          <t>log/eval_results_teacher_chronos-2_ctx720_pred96_exchange_rate_exchange_rate_20260114_224634.json</t>
         </is>
       </c>
     </row>
@@ -1350,12 +1350,12 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>20260113_092430</t>
+          <t>20260114_224717</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>log/eval_results_teacher_chronos-2_ctx720_pred96_illness_national_illness_20260113_092430.json</t>
+          <t>log/eval_results_teacher_chronos-2_ctx720_pred96_illness_national_illness_20260114_224717.json</t>
         </is>
       </c>
     </row>
@@ -1402,12 +1402,12 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>20260113_093124</t>
+          <t>20260114_225308</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>log/eval_results_teacher_chronos-2_ctx720_pred96_traffic_traffic_20260113_093124.json</t>
+          <t>log/eval_results_teacher_chronos-2_ctx720_pred96_traffic_traffic_20260114_225308.json</t>
         </is>
       </c>
     </row>
@@ -1456,12 +1456,12 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>20260113_093706</t>
+          <t>20260114_225856</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>log/eval_results_teacher_chronos-2_ctx720_pred96_weather_weather_20260113_093706.json</t>
+          <t>log/eval_results_teacher_chronos-2_ctx720_pred96_weather_weather_20260114_225856.json</t>
         </is>
       </c>
     </row>

</xml_diff>